<commit_message>
20171221 修正Google Excel問題單 第78 80 99條
</commit_message>
<xml_diff>
--- a/templates/組長歷史查詢結果.xlsx
+++ b/templates/組長歷史查詢結果.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>進口日期</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -95,6 +95,14 @@
   </si>
   <si>
     <t>${table:data.OL_REASON}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>改單人員</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.U_NAME}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -483,20 +491,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.25" customWidth="1"/>
-    <col min="5" max="9" width="13.5" customWidth="1"/>
+    <col min="5" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1">
+    <row r="1" spans="1:10" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -524,8 +532,11 @@
       <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -552,6 +563,9 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>